<commit_message>
Added one row per indicator and ecosystem
</commit_message>
<xml_diff>
--- a/indicators/NO_TCCD_001_104/metadata.xlsx
+++ b/indicators/NO_TCCD_001_104/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\61546-01_fu_intern_sylvie_clappe\ecRxiv_TCCD\TCCD\indicators\NO_TCCD_001_104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EA16D2-A66E-4C69-B19C-1059B4D2CC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A817DE37-27D7-4A69-B10D-A047CD2E7A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39525" yWindow="1125" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="-11640" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="217">
   <si>
     <t>Variable</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>Spatial aggregation pathway</t>
-  </si>
-  <si>
-    <t>Aggregation at small polygon scale within target area (TCCD area weighted mean) - Aggregation at target area scale (mean and standard error; city, region, national scales)</t>
   </si>
   <si>
     <t>Scale - [Transform, Truncate] - Aggregate</t>
@@ -704,14 +701,41 @@
     <t>TF1.7 Boreal/temperate fens</t>
   </si>
   <si>
-    <t>NO_TCCD_001-104</t>
+    <t>NO_NDVI_002</t>
+  </si>
+  <si>
+    <t>NO_NDVI_003</t>
+  </si>
+  <si>
+    <t>NO_NDVI_004</t>
+  </si>
+  <si>
+    <t>NO_NDVI_005</t>
+  </si>
+  <si>
+    <t>NO_TCCD_001</t>
+  </si>
+  <si>
+    <t>NO_TCCD_101</t>
+  </si>
+  <si>
+    <t>NO_TCCD_102</t>
+  </si>
+  <si>
+    <t>NO_TCCD_103</t>
+  </si>
+  <si>
+    <t>NO_TCCD_104</t>
+  </si>
+  <si>
+    <t>Aggregation at small polygon scale within target area (TCCD area weighted mean) - Aggregation at focal area scale (mean and standard error; city, region, national scales)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -763,6 +787,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -778,7 +808,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -825,6 +855,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -833,7 +876,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="4" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="4" applyBorder="1" applyProtection="1"/>
@@ -845,6 +888,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Excel Built-in Neutral" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -1251,21 +1296,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" customWidth="1"/>
-    <col min="3" max="3" width="106.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="2" max="2" width="47.88671875" customWidth="1"/>
+    <col min="3" max="3" width="106.44140625" customWidth="1"/>
     <col min="4" max="4" width="145" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1279,12 +1324,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>208</v>
+      <c r="B2" s="9" t="s">
+        <v>211</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>5</v>
@@ -1293,220 +1338,389 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B22" s="4">
         <v>2025</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B23" s="4">
         <v>2025</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B30" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>57</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C16" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B28" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1520,7 +1734,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B9</xm:sqref>
+          <xm:sqref>B17:B21</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -1529,7 +1743,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B7</xm:sqref>
+          <xm:sqref>B11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -1538,7 +1752,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B8</xm:sqref>
+          <xm:sqref>B12:B16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
@@ -1547,7 +1761,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B12</xm:sqref>
+          <xm:sqref>B24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
@@ -1556,7 +1770,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B17</xm:sqref>
+          <xm:sqref>B29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
@@ -1565,7 +1779,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B6</xm:sqref>
+          <xm:sqref>B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1581,15 +1795,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.6640625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1600,18 +1814,18 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
         <v>58</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
       </c>
       <c r="F1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -1623,24 +1837,24 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
         <v>61</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B3" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
@@ -1649,652 +1863,652 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>68</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>69</v>
       </c>
-      <c r="E4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
         <v>71</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>74</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>75</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>76</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>78</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>79</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>82</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>83</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>84</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>86</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>87</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>89</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>90</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>92</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>94</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>96</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>98</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>100</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>102</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>104</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>106</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>108</v>
       </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>110</v>
       </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>112</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>114</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>116</v>
       </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>118</v>
       </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>120</v>
       </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>122</v>
       </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D64" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D64" t="s">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" t="s">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" t="s">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D72" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D73" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D74" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D76" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D77" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D78" t="s">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D80" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D80" t="s">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" t="s">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D82" t="s">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" t="s">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" t="s">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D88" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D88" t="s">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D89" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D89" t="s">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D90" t="s">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D91" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D91" t="s">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D92" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D92" t="s">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D93" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D93" t="s">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D94" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D94" t="s">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D95" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D95" t="s">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D96" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D96" t="s">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" t="s">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D98" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D98" t="s">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D99" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" t="s">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D100" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D100" t="s">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D101" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D101" t="s">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D102" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D102" t="s">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D103" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D103" t="s">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D104" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D105" t="s">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D106" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D106" t="s">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D107" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D107" t="s">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D108" t="s">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D109" t="s">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D110" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D110" t="s">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D111" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D111" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>